<commit_message>
Add fig index to annotation for pairing with distortion metric
</commit_message>
<xml_diff>
--- a/data/misused_bar_graph_figures/bioeng_transl_med/log/annotation.xlsx
+++ b/data/misused_bar_graph_figures/bioeng_transl_med/log/annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Files/2023-2028-UC_Berkeley/_landry-lab/research-project/local/misused-bar-graphs/data/misused_bar_graph_figures/bioeng_transl_med/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3F9913-E14E-CF43-8479-96BF01733720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E570629-5D0E-FA47-9AED-5DD07C4C819C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="37620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19600" yWindow="500" windowWidth="18800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="53">
   <si>
     <t>DOI</t>
   </si>
@@ -140,6 +140,45 @@
   </si>
   <si>
     <t>Total radiant efficiency</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10634_log_fig1</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10602_log_fig1</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10594_log_fig4</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10594_log_fig3</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10594_log_fig2</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10594_log_fig1</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10538_log_fig2</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10538_log_fig1</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10514_log_fig2</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10514_log_fig1</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10487_log_fig2</t>
+  </si>
+  <si>
+    <t>10.1002:btm2.10487_log_fig1</t>
+  </si>
+  <si>
+    <t>Fig Index</t>
   </si>
 </sst>
 </file>
@@ -540,431 +579,470 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
       <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>31</v>
       </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
       <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>31</v>
       </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
       <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
       <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
         <v>38</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
       <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>39</v>
       </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
       <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
         <v>38</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
       <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
         <v>33</v>
       </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>39</v>
       </c>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
       <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
       <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>35</v>
       </c>
-      <c r="J12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
       <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
       <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>31</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>